<commit_message>
adding block design pictures\
</commit_message>
<xml_diff>
--- a/design-space-exploration/design-space-charts.xlsx
+++ b/design-space-exploration/design-space-charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schen\Documents\Spr 22\fpga\HWImageProcessor\design-space-exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F106175-110A-4340-A294-E7870A34E9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2F663-23A0-460E-9C1A-96F67386FBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-2754" windowWidth="23232" windowHeight="12432" xr2:uid="{31EA6664-D3C0-497B-BEA4-E9E786E423EB}"/>
   </bookViews>
@@ -204,12 +204,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Design Space</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Pareto graph</a:t>
+              <a:t>Pareto graph</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2262,9 +2258,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:colOff>41910</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2591,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883F8882-FFF4-4276-BF4D-193671C4D470}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
directory re-org and pareto picture
</commit_message>
<xml_diff>
--- a/design-space-exploration/design-space-charts.xlsx
+++ b/design-space-exploration/design-space-charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schen\Documents\Spr 22\fpga\HWImageProcessor\design-space-exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2F663-23A0-460E-9C1A-96F67386FBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87E4A5D-E894-4784-895A-2B1D8C6B3883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-2754" windowWidth="23232" windowHeight="12432" xr2:uid="{31EA6664-D3C0-497B-BEA4-E9E786E423EB}"/>
   </bookViews>
@@ -191,23 +191,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>Pareto graph</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -224,16 +223,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -268,16 +267,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -335,16 +335,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -402,16 +403,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -469,16 +471,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -536,16 +537,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent5"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -604,15 +604,16 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -670,20 +671,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -741,20 +739,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="dot"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -812,20 +809,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="dash"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent3">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -883,20 +879,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent4">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -954,20 +949,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1025,20 +1019,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent6">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1093,22 +1086,18 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:lumMod val="80000"/>
                     <a:lumOff val="20000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1166,22 +1155,18 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
                     <a:lumMod val="80000"/>
                     <a:lumOff val="20000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1240,21 +1225,19 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent3">
                     <a:lumMod val="80000"/>
                     <a:lumOff val="20000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1312,22 +1295,18 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="accent4">
                     <a:lumMod val="80000"/>
                     <a:lumOff val="20000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1385,7 +1364,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1402,9 +1381,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1434,9 +1413,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1458,9 +1437,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1474,7 +1454,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1502,7 +1482,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1519,9 +1499,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1551,9 +1531,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1575,9 +1555,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1591,7 +1572,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1609,7 +1590,17 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1617,7 +1608,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1633,7 +1624,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -1660,11 +1651,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1732,25 +1723,25 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1758,30 +1749,31 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1789,14 +1781,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -1833,37 +1825,49 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -1873,22 +1877,26 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -1912,16 +1920,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1929,14 +1936,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1947,9 +1954,9 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1961,12 +1968,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1980,14 +1987,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1999,13 +2006,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2013,12 +2027,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2032,14 +2046,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2051,14 +2065,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2070,12 +2084,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -2089,39 +2103,69 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2129,12 +2173,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -2147,13 +2191,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2162,14 +2206,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2178,7 +2221,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2190,7 +2233,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2198,9 +2241,9 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2212,7 +2255,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2220,9 +2263,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2235,13 +2279,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -2257,10 +2308,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>41910</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2587,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883F8882-FFF4-4276-BF4D-193671C4D470}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>